<commit_message>
added controller method for downloading WareHouseRequest
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/wareHouseRequest.xlsx
+++ b/src/main/resources/templates/wareHouseRequest.xlsx
@@ -309,7 +309,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,12 +323,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -339,64 +333,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -417,14 +357,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -433,27 +423,7 @@
     <cellStyle name="Обычный 2" xfId="1"/>
     <cellStyle name="Обычный_Лист1" xfId="2"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -789,8 +759,8 @@
   </sheetPr>
   <dimension ref="A2:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -804,15 +774,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="21">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="26" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="15.5">
       <c r="B3" s="1"/>
@@ -822,27 +792,27 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="26">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" ht="21">
       <c r="A5" s="2"/>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -851,7 +821,7 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -865,239 +835,239 @@
       <c r="A7" s="5">
         <v>1</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="6"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="5">
         <v>5</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="15.5">
       <c r="A11" s="5">
         <f t="shared" ref="A11:A22" si="0">A10+1</f>
         <v>6</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="15.5">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="8"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="20">
+      <c r="A17" s="11">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="20">
+      <c r="A18" s="11">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="20">
+      <c r="A19" s="11">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="20">
+      <c r="A20" s="11">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="20">
+      <c r="A21" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="20">
+      <c r="A22" s="11">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="37"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-    </row>
-    <row r="24" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A24" s="38" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="1:6" ht="17.5" customHeight="1">
+      <c r="A24" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-    </row>
-    <row r="25" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A25" s="40" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A25" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-    </row>
-    <row r="26" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A26" s="40" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" customHeight="1">
+      <c r="A26" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-    </row>
-    <row r="27" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A27" s="40" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1">
+      <c r="A27" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" spans="1:6" ht="36.75" customHeight="1">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="30" spans="1:6" ht="17">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6">
       <c r="C31" s="27" t="s">
@@ -1108,14 +1078,14 @@
       <c r="F31" s="27"/>
     </row>
     <row r="32" spans="1:6" ht="17">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6">
       <c r="C33" s="27" t="s">
@@ -1126,14 +1096,14 @@
       <c r="F33" s="27"/>
     </row>
     <row r="34" spans="1:6" ht="17">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6">
       <c r="C35" s="27" t="s">
@@ -1145,6 +1115,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="C35:F35"/>
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A4:F4"/>
@@ -1154,11 +1129,6 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="C35:F35"/>
   </mergeCells>
   <conditionalFormatting sqref="B28:B1048576 B11:B23 B1:B7">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>

</xml_diff>

<commit_message>
adding a column of wailable parts in wareHouseRequest
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/wareHouseRequest.xlsx
+++ b/src/main/resources/templates/wareHouseRequest.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>ООО" ИКО Машинери"</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Дата:</t>
+  </si>
+  <si>
+    <t>Сервисная Машина</t>
   </si>
 </sst>
 </file>
@@ -390,32 +393,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -757,10 +760,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F35"/>
+  <dimension ref="A2:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -774,15 +777,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="21">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6" ht="15.5">
       <c r="B3" s="1"/>
@@ -792,24 +795,24 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="26">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="21">
       <c r="A5" s="2"/>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
@@ -1021,122 +1024,133 @@
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
     </row>
-    <row r="25" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A25" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="36"/>
+    <row r="25" spans="1:6" ht="17.5" customHeight="1">
+      <c r="A25" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="35"/>
       <c r="C25" s="21"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="1:6" ht="18" customHeight="1">
-      <c r="A26" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="18"/>
+    <row r="26" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A26" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1">
-      <c r="A27" s="35" t="s">
+    <row r="27" spans="1:6" ht="18" customHeight="1">
+      <c r="A27" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="35"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1">
+      <c r="A28" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" ht="36.75" customHeight="1">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
     </row>
-    <row r="30" spans="1:6" ht="17">
-      <c r="A30" s="31" t="s">
+    <row r="29" spans="1:6" ht="36.75" customHeight="1">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+    </row>
+    <row r="31" spans="1:6" ht="17">
+      <c r="A31" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="C31" s="30" t="s">
-        <v>8</v>
-      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="30"/>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
     </row>
-    <row r="32" spans="1:6" ht="17">
-      <c r="A32" s="31" t="s">
+    <row r="32" spans="1:6">
+      <c r="C32" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+    </row>
+    <row r="33" spans="1:6" ht="17">
+      <c r="A33" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="C33" s="30" t="s">
-        <v>8</v>
-      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="30"/>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
     </row>
-    <row r="34" spans="1:6" ht="17">
-      <c r="A34" s="31" t="s">
+    <row r="34" spans="1:6">
+      <c r="C34" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+    </row>
+    <row r="35" spans="1:6" ht="17">
+      <c r="A35" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="C35" s="30" t="s">
-        <v>8</v>
-      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="30"/>
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
     </row>
+    <row r="36" spans="1:6">
+      <c r="C36" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A30:F30"/>
+  <mergeCells count="15">
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="A31:F31"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="B5:F5"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="C35:F35"/>
   </mergeCells>
-  <conditionalFormatting sqref="B28:B1048576 B11:B23 B1:B7">
+  <conditionalFormatting sqref="B29:B1048576 B11:B23 B1:B7">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
+  <conditionalFormatting sqref="B27">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>